<commit_message>
1. apps/es Bugfix. 2. apps/es add end-user manual.
</commit_message>
<xml_diff>
--- a/apps/es/resources/screen/ES004.xlsx
+++ b/apps/es/resources/screen/ES004.xlsx
@@ -1,33 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
-  <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\all-workspace\python\VsCodeProjects\wci2_es2\es\resources\screen\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B291C0FD-9E67-456B-B726-4E48DCE04F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1005" yWindow="-105" windowWidth="29040" windowHeight="4170"/>
   </bookViews>
   <sheets>
     <sheet name="View Dfn" sheetId="1" r:id="rId1"/>
     <sheet name="Widgets" sheetId="2" r:id="rId2"/>
     <sheet name="Notes" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="D18" authorId="0">
       <text>
         <r>
           <rPr>
@@ -46,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="290">
   <si>
     <t>Do not modify this column</t>
   </si>
@@ -223,6 +217,9 @@
   </si>
   <si>
     <t>availablePriorBalanceRcs</t>
+  </si>
+  <si>
+    <t>es.models.AvailablePriorBalance</t>
   </si>
   <si>
     <t>ccyRcs</t>
@@ -778,7 +775,7 @@
     <t>claimAmount</t>
   </si>
   <si>
-    <t>Cash advancement total avriable amount.</t>
+    <t>Cash advancement total available amount.</t>
   </si>
   <si>
     <t>total_amt</t>
@@ -790,7 +787,7 @@
     <t>Left</t>
   </si>
   <si>
-    <t>Avriable amount.</t>
+    <t>Available amount.</t>
   </si>
   <si>
     <t>balance_amt</t>
@@ -850,9 +847,6 @@
     <t>Download Supporting Document</t>
   </si>
   <si>
-    <t>icon: images/download_button.gif</t>
-  </si>
-  <si>
     <t>downloadSupportingDoc</t>
   </si>
   <si>
@@ -938,17 +932,14 @@
     <t>One tailor made javascript for each layout</t>
   </si>
   <si>
-    <t>es.models.AvailablePriorBalance</t>
-  </si>
-  <si>
-    <t>20250507122600</t>
+    <t>20250523115300</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1138,81 +1129,19 @@
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Normal 2 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Normal 2 2 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
-    <cellStyle name="Normal 2 3" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Normal 2 4" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Normal 2 5" xfId="9" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
-    <cellStyle name="Normal 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Normal 4" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Percent 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2 2" xfId="5"/>
+    <cellStyle name="Normal 2 2 2" xfId="8"/>
+    <cellStyle name="Normal 2 3" xfId="7"/>
+    <cellStyle name="Normal 2 4" xfId="4"/>
+    <cellStyle name="Normal 2 5" xfId="9"/>
+    <cellStyle name="Normal 3" xfId="6"/>
+    <cellStyle name="Normal 4" xfId="3"/>
+    <cellStyle name="Percent 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="1314450" y="1314450"/>
-          <a:ext cx="4772025" cy="4314825"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1499,15 +1428,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T117"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.28515625" style="7" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
@@ -1534,7 +1463,7 @@
     <col min="29" max="31" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="37.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1543,10 +1472,10 @@
       </c>
       <c r="D1" s="8"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" s="6"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1557,7 +1486,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15">
       <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
@@ -1570,7 +1499,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -1583,7 +1512,7 @@
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
@@ -1598,7 +1527,7 @@
       </c>
       <c r="E6" s="8"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
@@ -1613,7 +1542,7 @@
       </c>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8" s="6" t="s">
         <v>16</v>
       </c>
@@ -1626,7 +1555,7 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="A9" s="18" t="s">
         <v>19</v>
       </c>
@@ -1639,7 +1568,7 @@
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="A10" s="6" t="s">
         <v>22</v>
       </c>
@@ -1652,7 +1581,7 @@
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15">
       <c r="A11" s="6" t="s">
         <v>25</v>
       </c>
@@ -1663,7 +1592,7 @@
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15">
       <c r="A12" s="6" t="s">
         <v>27</v>
       </c>
@@ -1678,7 +1607,7 @@
       </c>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15">
       <c r="A13" s="6" t="s">
         <v>31</v>
       </c>
@@ -1691,7 +1620,7 @@
       </c>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="A14" s="6" t="s">
         <v>34</v>
       </c>
@@ -1699,14 +1628,14 @@
         <v>35</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E14" s="8"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15">
       <c r="A15" s="6" t="s">
         <v>37</v>
       </c>
@@ -1717,13 +1646,13 @@
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15">
       <c r="A16" s="6"/>
       <c r="I16" s="9"/>
       <c r="N16" s="9"/>
       <c r="O16" s="9"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20">
       <c r="A17" s="6"/>
       <c r="C17" s="9" t="s">
         <v>39</v>
@@ -1737,7 +1666,7 @@
       <c r="Q17" s="9"/>
       <c r="R17" s="9"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20">
       <c r="A18" s="6" t="s">
         <v>41</v>
       </c>
@@ -1766,7 +1695,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20">
       <c r="A19" s="6"/>
       <c r="C19" s="11" t="s">
         <v>49</v>
@@ -1782,7 +1711,7 @@
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20">
       <c r="C20" s="11" t="s">
         <v>52</v>
       </c>
@@ -1797,7 +1726,7 @@
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20">
       <c r="C21" s="11" t="s">
         <v>54</v>
       </c>
@@ -1812,7 +1741,7 @@
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20">
       <c r="C22" s="11" t="s">
         <v>56</v>
       </c>
@@ -1827,7 +1756,7 @@
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20">
       <c r="C23" s="11" t="s">
         <v>58</v>
       </c>
@@ -1835,68 +1764,68 @@
         <v>50</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>289</v>
+        <v>59</v>
       </c>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20">
       <c r="C24" s="11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F24" s="11"/>
       <c r="G24" s="11" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20">
       <c r="C25" s="11" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F25" s="11"/>
       <c r="G25" s="11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H25" s="11"/>
       <c r="I25" s="11"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20">
       <c r="C26" s="11" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D26" s="11" t="s">
         <v>50</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
       <c r="H26" s="11"/>
       <c r="I26" s="11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20">
       <c r="A27" s="6"/>
       <c r="C27" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -1905,117 +1834,117 @@
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20">
       <c r="A28" s="6"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20">
       <c r="A29" s="6"/>
       <c r="D29" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="S29" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20">
       <c r="A30" s="6"/>
       <c r="C30" s="9"/>
       <c r="D30" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="J30" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K30" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L30" s="9"/>
       <c r="M30" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N30" s="9"/>
       <c r="S30" s="9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20">
       <c r="A31" s="7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>28</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="N31" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="O31" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="P31" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="Q31" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="R31" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="S31" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="T31" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20">
       <c r="B32" s="1"/>
       <c r="C32" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E32" s="11"/>
       <c r="F32" s="11"/>
@@ -2030,7 +1959,7 @@
       <c r="M32" s="11"/>
       <c r="N32" s="11"/>
       <c r="O32" s="11" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="P32" s="11"/>
       <c r="Q32" s="11"/>
@@ -2038,12 +1967,12 @@
       <c r="S32" s="11"/>
       <c r="T32" s="11"/>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20">
       <c r="C33" s="11" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
@@ -2062,12 +1991,12 @@
       <c r="S33" s="11"/>
       <c r="T33" s="11"/>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20">
       <c r="C34" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D34" s="11" t="s">
         <v>100</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>99</v>
       </c>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
@@ -2083,20 +2012,20 @@
       <c r="P34" s="11"/>
       <c r="Q34" s="11"/>
       <c r="R34" s="11" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="S34" s="11"/>
       <c r="T34" s="11"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20">
       <c r="C35" s="11" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F35" s="11" t="s">
         <v>49</v>
@@ -2124,12 +2053,12 @@
       <c r="S35" s="11"/>
       <c r="T35" s="11"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20">
       <c r="C36" s="11" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
@@ -2150,15 +2079,15 @@
       <c r="S36" s="11"/>
       <c r="T36" s="11"/>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20">
       <c r="C37" s="11" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F37" s="11" t="s">
         <v>52</v>
@@ -2180,12 +2109,12 @@
       <c r="S37" s="11"/>
       <c r="T37" s="11"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20">
       <c r="C38" s="11" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E38" s="11"/>
       <c r="F38" s="11"/>
@@ -2206,16 +2135,16 @@
       <c r="S38" s="11"/>
       <c r="T38" s="11"/>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20">
       <c r="C39" s="11" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E39" s="11"/>
       <c r="F39" s="11" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G39" s="11"/>
       <c r="H39" s="11" t="s">
@@ -2234,15 +2163,15 @@
       <c r="S39" s="11"/>
       <c r="T39" s="11"/>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20">
       <c r="C40" s="11" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>58</v>
@@ -2266,12 +2195,12 @@
       <c r="S40" s="11"/>
       <c r="T40" s="11"/>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20">
       <c r="C41" s="11" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E41" s="11"/>
       <c r="F41" s="11"/>
@@ -2292,9 +2221,9 @@
       <c r="S41" s="11"/>
       <c r="T41" s="11"/>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20">
       <c r="C42" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
@@ -2314,90 +2243,90 @@
       <c r="S42" s="3"/>
       <c r="T42" s="3"/>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20">
       <c r="K44" s="9"/>
       <c r="M44" s="9"/>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20">
       <c r="C45" s="9"/>
       <c r="D45" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E45" s="9"/>
       <c r="F45" s="9"/>
       <c r="G45" s="9"/>
       <c r="H45" s="10" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I45" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J45" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="K45" s="10" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="M45" s="15"/>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20">
       <c r="A46" s="7" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H46" s="3" t="s">
         <v>28</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="K46" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="L46" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="M46" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="N46" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O46" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="P46" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20">
       <c r="B47" s="1"/>
       <c r="C47" s="11" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D47" s="11"/>
       <c r="E47" s="11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F47" s="11"/>
       <c r="G47" s="11"/>
@@ -2405,23 +2334,23 @@
       <c r="I47" s="11"/>
       <c r="J47" s="11"/>
       <c r="K47" s="11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="L47" s="11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="M47" s="11" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="N47" s="11"/>
       <c r="O47" s="11"/>
       <c r="P47" s="11"/>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20">
       <c r="C48" s="11"/>
       <c r="D48" s="11"/>
       <c r="E48" s="11" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F48" s="11"/>
       <c r="G48" s="11"/>
@@ -2429,21 +2358,21 @@
       <c r="I48" s="11"/>
       <c r="J48" s="11"/>
       <c r="K48" s="11" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="L48" s="11"/>
       <c r="M48" s="11" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="N48" s="11"/>
       <c r="O48" s="11"/>
       <c r="P48" s="11"/>
     </row>
-    <row r="49" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:16">
       <c r="C49" s="11"/>
       <c r="D49" s="11"/>
       <c r="E49" s="11" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F49" s="11"/>
       <c r="G49" s="11"/>
@@ -2451,49 +2380,49 @@
       <c r="I49" s="11"/>
       <c r="J49" s="11"/>
       <c r="K49" s="11" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="L49" s="11" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="M49" s="11" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="N49" s="11"/>
       <c r="O49" s="11"/>
       <c r="P49" s="11"/>
     </row>
-    <row r="50" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:16">
       <c r="C50" s="11"/>
       <c r="D50" s="11"/>
       <c r="E50" s="11" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F50" s="11" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G50" s="11"/>
       <c r="H50" s="11"/>
       <c r="I50" s="11"/>
       <c r="J50" s="11"/>
       <c r="K50" s="11" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="L50" s="11" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="M50" s="11" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="N50" s="11"/>
       <c r="O50" s="11"/>
       <c r="P50" s="11"/>
     </row>
-    <row r="51" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:16">
       <c r="C51" s="11"/>
       <c r="D51" s="11"/>
       <c r="E51" s="11" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F51" s="11"/>
       <c r="G51" s="11"/>
@@ -2501,73 +2430,73 @@
       <c r="I51" s="11"/>
       <c r="J51" s="11"/>
       <c r="K51" s="11" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="L51" s="11" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="M51" s="11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="N51" s="11"/>
       <c r="O51" s="11" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="P51" s="11"/>
     </row>
-    <row r="52" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:16">
       <c r="C52" s="11"/>
       <c r="D52" s="11"/>
       <c r="E52" s="11" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F52" s="11" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G52" s="11"/>
       <c r="H52" s="11"/>
       <c r="I52" s="11"/>
       <c r="J52" s="11"/>
       <c r="K52" s="11" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="L52" s="11"/>
       <c r="M52" s="11" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="N52" s="11"/>
       <c r="O52" s="11"/>
       <c r="P52" s="11"/>
     </row>
-    <row r="53" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:16">
       <c r="C53" s="11"/>
       <c r="D53" s="11"/>
       <c r="E53" s="11" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F53" s="11" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G53" s="11"/>
       <c r="H53" s="11"/>
       <c r="I53" s="11"/>
       <c r="J53" s="11"/>
       <c r="K53" s="11" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="L53" s="11"/>
       <c r="M53" s="11" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="N53" s="11"/>
       <c r="O53" s="11"/>
       <c r="P53" s="11"/>
     </row>
-    <row r="54" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:16">
       <c r="C54" s="11"/>
       <c r="D54" s="11"/>
       <c r="E54" s="11" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F54" s="11"/>
       <c r="G54" s="11"/>
@@ -2575,73 +2504,73 @@
       <c r="I54" s="11"/>
       <c r="J54" s="11"/>
       <c r="K54" s="11" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="L54" s="11" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M54" s="11" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="N54" s="11"/>
       <c r="O54" s="11"/>
       <c r="P54" s="11"/>
     </row>
-    <row r="55" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:16">
       <c r="C55" s="11"/>
       <c r="D55" s="11"/>
       <c r="E55" s="11"/>
       <c r="F55" s="11" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="G55" s="11"/>
       <c r="H55" s="11"/>
       <c r="I55" s="11"/>
       <c r="J55" s="11"/>
       <c r="K55" s="11" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="L55" s="11" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="M55" s="11"/>
       <c r="N55" s="11" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="O55" s="11"/>
       <c r="P55" s="11"/>
     </row>
-    <row r="56" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:16">
       <c r="C56" s="11"/>
       <c r="D56" s="11"/>
       <c r="E56" s="11"/>
       <c r="F56" s="11" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G56" s="11"/>
       <c r="H56" s="11"/>
       <c r="I56" s="11"/>
       <c r="J56" s="11"/>
       <c r="K56" s="11" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="L56" s="11"/>
       <c r="M56" s="11"/>
       <c r="N56" s="11" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="O56" s="11"/>
       <c r="P56" s="11"/>
     </row>
-    <row r="57" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:16">
       <c r="C57" s="11" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F57" s="11"/>
       <c r="G57" s="11"/>
@@ -2649,27 +2578,27 @@
       <c r="I57" s="11"/>
       <c r="J57" s="11"/>
       <c r="K57" s="11" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="L57" s="11" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="M57" s="11"/>
       <c r="N57" s="11" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="O57" s="11"/>
       <c r="P57" s="11"/>
     </row>
-    <row r="58" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:16">
       <c r="C58" s="11" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F58" s="11"/>
       <c r="G58" s="11"/>
@@ -2677,23 +2606,23 @@
       <c r="I58" s="11"/>
       <c r="J58" s="11"/>
       <c r="K58" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="L58" s="11"/>
       <c r="M58" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="N58" s="11"/>
       <c r="O58" s="11"/>
       <c r="P58" s="11"/>
     </row>
-    <row r="59" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:16">
       <c r="C59" s="11"/>
       <c r="D59" s="11" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E59" s="11" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F59" s="11"/>
       <c r="G59" s="11"/>
@@ -2701,23 +2630,23 @@
       <c r="I59" s="11"/>
       <c r="J59" s="11"/>
       <c r="K59" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="L59" s="11"/>
       <c r="M59" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="N59" s="11"/>
       <c r="O59" s="11"/>
       <c r="P59" s="11"/>
     </row>
-    <row r="60" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:16">
       <c r="C60" s="11"/>
       <c r="D60" s="11" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E60" s="11" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F60" s="11"/>
       <c r="G60" s="11"/>
@@ -2725,131 +2654,131 @@
       <c r="I60" s="11"/>
       <c r="J60" s="11"/>
       <c r="K60" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="L60" s="11" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="M60" s="11" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="N60" s="11"/>
       <c r="O60" s="11" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="P60" s="11"/>
     </row>
-    <row r="61" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:16">
       <c r="C61" s="11"/>
       <c r="D61" s="11" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E61" s="11"/>
       <c r="F61" s="11" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="G61" s="11"/>
       <c r="H61" s="11"/>
       <c r="I61" s="11"/>
       <c r="J61" s="11"/>
       <c r="K61" s="11" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="L61" s="11" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="M61" s="11"/>
       <c r="N61" s="11" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="O61" s="11"/>
       <c r="P61" s="11"/>
     </row>
-    <row r="62" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:16">
       <c r="C62" s="11"/>
       <c r="D62" s="11" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E62" s="11"/>
       <c r="F62" s="11" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G62" s="11"/>
       <c r="H62" s="11"/>
       <c r="I62" s="11"/>
       <c r="J62" s="11"/>
       <c r="K62" s="11" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="L62" s="11" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="M62" s="11"/>
       <c r="N62" s="11" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="O62" s="11"/>
       <c r="P62" s="11"/>
     </row>
-    <row r="63" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:16">
       <c r="C63" s="11"/>
       <c r="D63" s="11" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E63" s="11"/>
       <c r="F63" s="11" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G63" s="11"/>
       <c r="H63" s="11"/>
       <c r="I63" s="11"/>
       <c r="J63" s="11"/>
       <c r="K63" s="11" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="L63" s="11" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="M63" s="11"/>
       <c r="N63" s="11" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="O63" s="11"/>
       <c r="P63" s="11"/>
     </row>
-    <row r="64" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:16">
       <c r="C64" s="11"/>
       <c r="D64" s="11" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E64" s="11"/>
       <c r="F64" s="11" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G64" s="11"/>
       <c r="H64" s="11"/>
       <c r="I64" s="11"/>
       <c r="J64" s="11"/>
       <c r="K64" s="11" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="L64" s="11"/>
       <c r="M64" s="11"/>
       <c r="N64" s="11" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="O64" s="11"/>
       <c r="P64" s="11"/>
     </row>
-    <row r="65" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:16">
       <c r="C65" s="11" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F65" s="11"/>
       <c r="G65" s="11"/>
@@ -2857,25 +2786,25 @@
       <c r="I65" s="11"/>
       <c r="J65" s="11"/>
       <c r="K65" s="11" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="L65" s="11" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="M65" s="11"/>
       <c r="N65" s="11" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="O65" s="11"/>
       <c r="P65" s="11"/>
     </row>
-    <row r="66" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:16">
       <c r="C66" s="11"/>
       <c r="D66" s="11" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F66" s="11"/>
       <c r="G66" s="11" t="s">
@@ -2885,27 +2814,27 @@
       <c r="I66" s="11"/>
       <c r="J66" s="11"/>
       <c r="K66" s="11" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="L66" s="11" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="M66" s="11"/>
       <c r="N66" s="11" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="O66" s="11"/>
       <c r="P66" s="11"/>
     </row>
-    <row r="67" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:16">
       <c r="C67" s="11" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D67" s="11" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F67" s="11"/>
       <c r="G67" s="11"/>
@@ -2913,7 +2842,7 @@
       <c r="I67" s="11"/>
       <c r="J67" s="11"/>
       <c r="K67" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="L67" s="11"/>
       <c r="M67" s="11"/>
@@ -2921,13 +2850,13 @@
       <c r="O67" s="11"/>
       <c r="P67" s="11"/>
     </row>
-    <row r="68" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:16">
       <c r="C68" s="11"/>
       <c r="D68" s="11" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E68" s="11" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F68" s="11"/>
       <c r="G68" s="11"/>
@@ -2935,7 +2864,7 @@
       <c r="I68" s="11"/>
       <c r="J68" s="11"/>
       <c r="K68" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="L68" s="11"/>
       <c r="M68" s="11"/>
@@ -2943,13 +2872,13 @@
       <c r="O68" s="11"/>
       <c r="P68" s="11"/>
     </row>
-    <row r="69" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:16">
       <c r="C69" s="11"/>
       <c r="D69" s="11" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F69" s="11"/>
       <c r="G69" s="11"/>
@@ -2957,23 +2886,23 @@
       <c r="I69" s="11"/>
       <c r="J69" s="11"/>
       <c r="K69" s="11" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="L69" s="11"/>
       <c r="M69" s="11"/>
       <c r="N69" s="11"/>
       <c r="O69" s="11" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="P69" s="11"/>
     </row>
-    <row r="70" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:16">
       <c r="C70" s="11"/>
       <c r="D70" s="11" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E70" s="11" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F70" s="11"/>
       <c r="G70" s="11"/>
@@ -2981,25 +2910,25 @@
       <c r="I70" s="11"/>
       <c r="J70" s="11"/>
       <c r="K70" s="11" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="L70" s="11" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="M70" s="11"/>
       <c r="N70" s="11"/>
       <c r="O70" s="11" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="P70" s="11"/>
     </row>
-    <row r="71" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:16">
       <c r="C71" s="11"/>
       <c r="D71" s="11" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E71" s="11" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F71" s="11"/>
       <c r="G71" s="11"/>
@@ -3007,25 +2936,25 @@
       <c r="I71" s="11"/>
       <c r="J71" s="11"/>
       <c r="K71" s="11" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="L71" s="11" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="M71" s="11"/>
       <c r="N71" s="11"/>
       <c r="O71" s="11" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="P71" s="11"/>
     </row>
-    <row r="72" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:16">
       <c r="C72" s="11"/>
       <c r="D72" s="11" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E72" s="11" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="F72" s="11"/>
       <c r="G72" s="11"/>
@@ -3035,25 +2964,25 @@
         <v>29</v>
       </c>
       <c r="K72" s="11" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="L72" s="11" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="M72" s="11"/>
       <c r="N72" s="11"/>
       <c r="O72" s="11" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="P72" s="11"/>
     </row>
-    <row r="73" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:16">
       <c r="C73" s="11"/>
       <c r="D73" s="11" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E73" s="11" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F73" s="11"/>
       <c r="G73" s="11"/>
@@ -3061,7 +2990,7 @@
       <c r="I73" s="11"/>
       <c r="J73" s="11"/>
       <c r="K73" s="11" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L73" s="11"/>
       <c r="M73" s="11"/>
@@ -3069,13 +2998,13 @@
       <c r="O73" s="11"/>
       <c r="P73" s="11"/>
     </row>
-    <row r="74" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:16">
       <c r="C74" s="11"/>
       <c r="D74" s="11" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="F74" s="11"/>
       <c r="G74" s="11"/>
@@ -3085,22 +3014,22 @@
         <v>29</v>
       </c>
       <c r="K74" s="11" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="L74" s="11" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="M74" s="11"/>
       <c r="N74" s="11"/>
       <c r="O74" s="11" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="P74" s="11"/>
     </row>
-    <row r="75" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:16">
       <c r="C75" s="11"/>
       <c r="D75" s="11" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E75" s="11" t="s">
         <v>11</v>
@@ -3111,23 +3040,23 @@
       <c r="I75" s="11"/>
       <c r="J75" s="11"/>
       <c r="K75" s="11" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="L75" s="11"/>
       <c r="M75" s="11"/>
       <c r="N75" s="11"/>
       <c r="O75" s="11" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="P75" s="11"/>
     </row>
-    <row r="76" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:16">
       <c r="C76" s="11"/>
       <c r="D76" s="11" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F76" s="11"/>
       <c r="G76" s="11"/>
@@ -3135,7 +3064,7 @@
       <c r="I76" s="11"/>
       <c r="J76" s="11"/>
       <c r="K76" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="L76" s="11"/>
       <c r="M76" s="11"/>
@@ -3143,125 +3072,125 @@
       <c r="O76" s="11"/>
       <c r="P76" s="11"/>
     </row>
-    <row r="77" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:16">
       <c r="C77" s="11" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E77" s="11" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="F77" s="11" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="G77" s="11"/>
       <c r="H77" s="11" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="I77" s="11"/>
       <c r="J77" s="11"/>
       <c r="K77" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="L77" s="11"/>
       <c r="M77" s="11" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="N77" s="11"/>
       <c r="O77" s="11"/>
       <c r="P77" s="11"/>
     </row>
-    <row r="78" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:16">
       <c r="C78" s="11"/>
       <c r="D78" s="11" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E78" s="11" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F78" s="11"/>
       <c r="G78" s="11"/>
       <c r="H78" s="11" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="I78" s="11"/>
       <c r="J78" s="11"/>
       <c r="K78" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="L78" s="11"/>
       <c r="M78" s="11" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="N78" s="11"/>
       <c r="O78" s="11"/>
       <c r="P78" s="11"/>
     </row>
-    <row r="79" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:16">
       <c r="C79" s="11"/>
       <c r="D79" s="11" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E79" s="11" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F79" s="11" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G79" s="11"/>
       <c r="H79" s="11" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="I79" s="11"/>
       <c r="J79" s="11"/>
       <c r="K79" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="L79" s="11"/>
       <c r="M79" s="11" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="N79" s="11"/>
       <c r="O79" s="11"/>
       <c r="P79" s="11"/>
     </row>
-    <row r="80" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:16">
       <c r="C80" s="11"/>
       <c r="D80" s="11" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E80" s="11" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F80" s="11" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="G80" s="11"/>
       <c r="H80" s="11" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="I80" s="11"/>
       <c r="J80" s="11"/>
       <c r="K80" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="L80" s="11"/>
       <c r="M80" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N80" s="11"/>
       <c r="O80" s="11"/>
       <c r="P80" s="11"/>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16">
       <c r="C81" s="11"/>
       <c r="D81" s="11" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E81" s="11" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F81" s="11"/>
       <c r="G81" s="11"/>
@@ -3269,25 +3198,25 @@
       <c r="I81" s="11"/>
       <c r="J81" s="11"/>
       <c r="K81" s="11" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="L81" s="11"/>
       <c r="M81" s="11" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="N81" s="11"/>
       <c r="O81" s="11"/>
       <c r="P81" s="11"/>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16">
       <c r="C82" s="11" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D82" s="11" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E82" s="11" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F82" s="11"/>
       <c r="G82" s="11"/>
@@ -3295,25 +3224,25 @@
       <c r="I82" s="11"/>
       <c r="J82" s="11"/>
       <c r="K82" s="11" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="L82" s="11" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="M82" s="11"/>
       <c r="N82" s="11" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="O82" s="11"/>
       <c r="P82" s="11"/>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16">
       <c r="C83" s="11"/>
       <c r="D83" s="11" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="E83" s="11" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="F83" s="11"/>
       <c r="G83" s="11"/>
@@ -3321,25 +3250,25 @@
       <c r="I83" s="11"/>
       <c r="J83" s="11"/>
       <c r="K83" s="11" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="L83" s="11" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="M83" s="11"/>
       <c r="N83" s="11" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="O83" s="11"/>
       <c r="P83" s="11"/>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16">
       <c r="C84" s="11"/>
       <c r="D84" s="11" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E84" s="11" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F84" s="11"/>
       <c r="G84" s="11"/>
@@ -3347,25 +3276,25 @@
       <c r="I84" s="11"/>
       <c r="J84" s="11"/>
       <c r="K84" s="11" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="L84" s="11" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="M84" s="11"/>
       <c r="N84" s="11" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="O84" s="11"/>
       <c r="P84" s="11"/>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16">
       <c r="C85" s="11"/>
       <c r="D85" s="11" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="E85" s="11" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F85" s="11"/>
       <c r="G85" s="11"/>
@@ -3373,10 +3302,10 @@
       <c r="I85" s="11"/>
       <c r="J85" s="11"/>
       <c r="K85" s="11" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="L85" s="11" t="s">
-        <v>260</v>
+        <v>191</v>
       </c>
       <c r="M85" s="11"/>
       <c r="N85" s="11" t="s">
@@ -3385,7 +3314,7 @@
       <c r="O85" s="11"/>
       <c r="P85" s="11"/>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16">
       <c r="C86" s="11"/>
       <c r="D86" s="11" t="s">
         <v>262</v>
@@ -3399,7 +3328,7 @@
       <c r="I86" s="11"/>
       <c r="J86" s="11"/>
       <c r="K86" s="11" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="L86" s="11" t="s">
         <v>264</v>
@@ -3411,9 +3340,9 @@
       <c r="O86" s="11"/>
       <c r="P86" s="11"/>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16">
       <c r="C87" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D87" s="3"/>
       <c r="E87" s="3"/>
@@ -3429,7 +3358,7 @@
       <c r="O87" s="3"/>
       <c r="P87" s="3"/>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16">
       <c r="A91" s="7" t="s">
         <v>266</v>
       </c>
@@ -3440,13 +3369,13 @@
         <v>268</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16">
       <c r="C92" s="11" t="s">
         <v>269</v>
       </c>
@@ -3455,17 +3384,17 @@
       </c>
       <c r="E92" s="11"/>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16">
       <c r="C93" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16">
       <c r="B96" s="1"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11">
       <c r="A97" s="7" t="s">
         <v>271</v>
       </c>
@@ -3473,7 +3402,7 @@
         <v>272</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D97" s="3" t="s">
         <v>273</v>
@@ -3488,23 +3417,23 @@
         <v>38</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11">
       <c r="C98" s="11"/>
       <c r="D98" s="11"/>
       <c r="E98" s="11"/>
       <c r="F98" s="11"/>
       <c r="G98" s="11"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11">
       <c r="C99" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D99" s="3"/>
       <c r="E99" s="3"/>
       <c r="F99" s="3"/>
       <c r="G99" s="3"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11">
       <c r="B102" s="16" t="s">
         <v>276</v>
       </c>
@@ -3512,16 +3441,16 @@
         <v>277</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11">
       <c r="A103" s="12" t="s">
         <v>278</v>
       </c>
       <c r="B103" s="13"/>
       <c r="C103" s="17" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D103" s="17" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E103" s="17" t="s">
         <v>279</v>
@@ -3542,15 +3471,15 @@
         <v>283</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11">
       <c r="C104" s="11" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D104" s="11" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E104" s="11" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F104" s="11"/>
       <c r="G104" s="11"/>
@@ -3560,13 +3489,13 @@
         <v>284</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11">
       <c r="C105" s="11"/>
       <c r="D105" s="11" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E105" s="11" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F105" s="11"/>
       <c r="G105" s="11"/>
@@ -3575,13 +3504,13 @@
       </c>
       <c r="I105" s="11"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11">
       <c r="C106" s="11"/>
       <c r="D106" s="11" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E106" s="11" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F106" s="11"/>
       <c r="G106" s="11"/>
@@ -3590,10 +3519,10 @@
       </c>
       <c r="I106" s="11"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11">
       <c r="C107" s="11"/>
       <c r="D107" s="11" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E107" s="11"/>
       <c r="F107" s="11"/>
@@ -3601,10 +3530,10 @@
       <c r="H107" s="11"/>
       <c r="I107" s="11"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11">
       <c r="C108" s="11"/>
       <c r="D108" s="11" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E108" s="11"/>
       <c r="F108" s="11"/>
@@ -3612,10 +3541,10 @@
       <c r="H108" s="11"/>
       <c r="I108" s="11"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11">
       <c r="C109" s="11"/>
       <c r="D109" s="11" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E109" s="11"/>
       <c r="F109" s="11"/>
@@ -3623,10 +3552,10 @@
       <c r="H109" s="11"/>
       <c r="I109" s="11"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11">
       <c r="C110" s="11"/>
       <c r="D110" s="11" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E110" s="11"/>
       <c r="F110" s="11"/>
@@ -3634,28 +3563,28 @@
       <c r="H110" s="11"/>
       <c r="I110" s="11"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11">
       <c r="C111" s="11" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D111" s="11" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E111" s="11" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="F111" s="11"/>
       <c r="G111" s="11"/>
       <c r="H111" s="11"/>
       <c r="I111" s="11"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11">
       <c r="C112" s="11"/>
       <c r="D112" s="11" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E112" s="11" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F112" s="11"/>
       <c r="G112" s="11"/>
@@ -3664,13 +3593,13 @@
       </c>
       <c r="I112" s="11"/>
     </row>
-    <row r="113" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:9">
       <c r="C113" s="11"/>
       <c r="D113" s="11" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E113" s="11" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F113" s="11"/>
       <c r="G113" s="11"/>
@@ -3679,13 +3608,13 @@
       </c>
       <c r="I113" s="11"/>
     </row>
-    <row r="114" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:9">
       <c r="C114" s="11"/>
       <c r="D114" s="11" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E114" s="11" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F114" s="11"/>
       <c r="G114" s="11"/>
@@ -3694,13 +3623,13 @@
       </c>
       <c r="I114" s="11"/>
     </row>
-    <row r="115" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:9">
       <c r="C115" s="11"/>
       <c r="D115" s="11" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E115" s="11" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F115" s="11"/>
       <c r="G115" s="11"/>
@@ -3709,9 +3638,9 @@
       </c>
       <c r="I115" s="11"/>
     </row>
-    <row r="116" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:9">
       <c r="C116" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D116" s="3"/>
       <c r="E116" s="3"/>
@@ -3720,7 +3649,7 @@
       <c r="H116" s="3"/>
       <c r="I116" s="3"/>
     </row>
-    <row r="117" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="3:9">
       <c r="H117" s="8"/>
     </row>
   </sheetData>
@@ -3731,20 +3660,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A5:C32"/>
   <sheetViews>
@@ -3752,12 +3681,12 @@
       <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -3765,18 +3694,17 @@
         <v>288</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1">
       <c r="A32">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>